<commit_message>
changed managers to allow chart and admin
</commit_message>
<xml_diff>
--- a/examples/assessmydeal-example-5556.xlsx
+++ b/examples/assessmydeal-example-5556.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="279">
   <si>
     <t>Question</t>
   </si>
@@ -854,13 +854,19 @@
   </si>
   <si>
     <t>example_survey</t>
+  </si>
+  <si>
+    <t>surveyor@highlandsnegotiations.com</t>
+  </si>
+  <si>
+    <t>Highlands@Survey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -989,6 +995,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1342,7 +1355,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1453,6 +1466,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="321">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2112,10 +2126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2192,6 +2206,17 @@
       <c r="B6" s="21"/>
       <c r="C6" s="29" t="s">
         <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>